<commit_message>
core: add .gitignore file and some new resoultion test files
all python compiled code is not tracked anymore and some other editor computer speicific log files
will be ignored during the push/pull processes
</commit_message>
<xml_diff>
--- a/scripts/ParameterTests/resolution/resolution_RESULTS.xlsx
+++ b/scripts/ParameterTests/resolution/resolution_RESULTS.xlsx
@@ -13,7 +13,11 @@
   </bookViews>
   <sheets>
     <sheet name="ResolutionTests" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Reactor_r10_analysis" localSheetId="1">Tabelle1!$A$1:$C$99</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,8 +27,20 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="Reactor_r10_analysis" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\sassibub\modOpt\scripts\ParameterTests\resolution\resolution_1_RESULTS\Reactor_r10_analysis.txt" thousands=".">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="130">
   <si>
     <t>Model</t>
   </si>
@@ -117,6 +133,303 @@
   </si>
   <si>
     <t>3, 3</t>
+  </si>
+  <si>
+    <t>***** Results of Analysis *****</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>VarBounds_0</t>
+  </si>
+  <si>
+    <t>VarBoundFraction</t>
+  </si>
+  <si>
+    <t>e0_h_SecRfeed_c1</t>
+  </si>
+  <si>
+    <t>e0_h_SecRfeed_c2</t>
+  </si>
+  <si>
+    <t>e0_h_SecRfeed_c3</t>
+  </si>
+  <si>
+    <t>e0_h_SecRfeed_c4</t>
+  </si>
+  <si>
+    <t>e0_h_SecRfeed_c5</t>
+  </si>
+  <si>
+    <t>e0_HU_LSecR</t>
+  </si>
+  <si>
+    <t>e0_v_LSecR</t>
+  </si>
+  <si>
+    <t>e0_greek_epsiv_LSecR</t>
+  </si>
+  <si>
+    <t>e0_V_SecRV</t>
+  </si>
+  <si>
+    <t>e0_HU_SecRV</t>
+  </si>
+  <si>
+    <t>e0_v_SecRV</t>
+  </si>
+  <si>
+    <t>e0_c_SecR_c1</t>
+  </si>
+  <si>
+    <t>e0_c_SecR_c2</t>
+  </si>
+  <si>
+    <t>e0_greek_DeltaP_SecR</t>
+  </si>
+  <si>
+    <t>e0_P_SecR</t>
+  </si>
+  <si>
+    <t>e0_greek_rho_LSecR</t>
+  </si>
+  <si>
+    <t>e0_M_LSecR</t>
+  </si>
+  <si>
+    <t>e0_greek_rho_SecRV</t>
+  </si>
+  <si>
+    <t>e0_M_SecRV</t>
+  </si>
+  <si>
+    <t>e0_greek_alpha_SecR_c1</t>
+  </si>
+  <si>
+    <t>e0_greek_alpha_SecR_c2</t>
+  </si>
+  <si>
+    <t>e0_greek_alpha_SecR_c3</t>
+  </si>
+  <si>
+    <t>e0_greek_alpha_SecR_c4</t>
+  </si>
+  <si>
+    <t>e0_greek_alpha_SecR_c5</t>
+  </si>
+  <si>
+    <t>e0_a_c1</t>
+  </si>
+  <si>
+    <t>e0_a_c2</t>
+  </si>
+  <si>
+    <t>e0_a_c3</t>
+  </si>
+  <si>
+    <t>e0_a_c4</t>
+  </si>
+  <si>
+    <t>e0_a_c5</t>
+  </si>
+  <si>
+    <t>e0_a_LSecR</t>
+  </si>
+  <si>
+    <t>e0_a_SecRV</t>
+  </si>
+  <si>
+    <t>e0_b_c1</t>
+  </si>
+  <si>
+    <t>e0_b_c2</t>
+  </si>
+  <si>
+    <t>e0_b_c3</t>
+  </si>
+  <si>
+    <t>e0_b_c4</t>
+  </si>
+  <si>
+    <t>e0_b_c5</t>
+  </si>
+  <si>
+    <t>e0_b_LSecR</t>
+  </si>
+  <si>
+    <t>e0_b_SecRV</t>
+  </si>
+  <si>
+    <t>e0_m_c1</t>
+  </si>
+  <si>
+    <t>e0_m_c2</t>
+  </si>
+  <si>
+    <t>e0_m_c3</t>
+  </si>
+  <si>
+    <t>e0_m_c4</t>
+  </si>
+  <si>
+    <t>e0_m_c5</t>
+  </si>
+  <si>
+    <t>e0_F_LSecR_c1</t>
+  </si>
+  <si>
+    <t>e0_F_LSecR_c2</t>
+  </si>
+  <si>
+    <t>e0_F_LSecR_c3</t>
+  </si>
+  <si>
+    <t>e0_F_LSecR_c4</t>
+  </si>
+  <si>
+    <t>e0_F_LSecR_c5</t>
+  </si>
+  <si>
+    <t>e0_F_SecRV_c1</t>
+  </si>
+  <si>
+    <t>e0_F_SecRV_c2</t>
+  </si>
+  <si>
+    <t>e0_F_SecRV_c3</t>
+  </si>
+  <si>
+    <t>e0_F_SecRV_c4</t>
+  </si>
+  <si>
+    <t>e0_F_SecRV_c5</t>
+  </si>
+  <si>
+    <t>e0_V_LSecR</t>
+  </si>
+  <si>
+    <t>e0_r_SecR_r1</t>
+  </si>
+  <si>
+    <t>e0_r_SecR_r2</t>
+  </si>
+  <si>
+    <t>e0_greek_phiv_LSecR_c1</t>
+  </si>
+  <si>
+    <t>e0_greek_phiv_LSecR_c2</t>
+  </si>
+  <si>
+    <t>e0_greek_phiv_LSecR_c3</t>
+  </si>
+  <si>
+    <t>e0_greek_phiv_LSecR_c4</t>
+  </si>
+  <si>
+    <t>e0_greek_phiv_LSecR_c5</t>
+  </si>
+  <si>
+    <t>e0_greek_phiv_SecRV_c1</t>
+  </si>
+  <si>
+    <t>e0_greek_phiv_SecRV_c2</t>
+  </si>
+  <si>
+    <t>e0_greek_phiv_SecRV_c3</t>
+  </si>
+  <si>
+    <t>e0_greek_phiv_SecRV_c4</t>
+  </si>
+  <si>
+    <t>e0_greek_phiv_SecRV_c5</t>
+  </si>
+  <si>
+    <t>e0_F_SecRV</t>
+  </si>
+  <si>
+    <t>e0_F_SecRfeed</t>
+  </si>
+  <si>
+    <t>e0_HU_LSecR_c1</t>
+  </si>
+  <si>
+    <t>e0_HU_LSecR_c2</t>
+  </si>
+  <si>
+    <t>e0_HU_LSecR_c3</t>
+  </si>
+  <si>
+    <t>e0_HU_LSecR_c4</t>
+  </si>
+  <si>
+    <t>e0_HU_LSecR_c5</t>
+  </si>
+  <si>
+    <t>e0_HU_SecR_c1</t>
+  </si>
+  <si>
+    <t>e0_HU_SecR_c2</t>
+  </si>
+  <si>
+    <t>e0_HU_SecR_c3</t>
+  </si>
+  <si>
+    <t>e0_HU_SecR_c4</t>
+  </si>
+  <si>
+    <t>e0_HU_SecR_c5</t>
+  </si>
+  <si>
+    <t>e0_HU_SecRV_c1</t>
+  </si>
+  <si>
+    <t>e0_HU_SecRV_c2</t>
+  </si>
+  <si>
+    <t>e0_HU_SecRV_c3</t>
+  </si>
+  <si>
+    <t>e0_HU_SecRV_c4</t>
+  </si>
+  <si>
+    <t>e0_HU_SecRV_c5</t>
+  </si>
+  <si>
+    <t>e0_h_LSecR</t>
+  </si>
+  <si>
+    <t>e0_h_SecRV</t>
+  </si>
+  <si>
+    <t>e0_h_SecRfeed</t>
+  </si>
+  <si>
+    <t>e0_greek_Deltah_SecRVLdeparture</t>
+  </si>
+  <si>
+    <t>e0_h_SecRV_c1</t>
+  </si>
+  <si>
+    <t>e0_h_SecRV_c2</t>
+  </si>
+  <si>
+    <t>e0_h_SecRV_c3</t>
+  </si>
+  <si>
+    <t>e0_h_SecRV_c4</t>
+  </si>
+  <si>
+    <t>e0_h_SecRV_c5</t>
+  </si>
+  <si>
+    <t>e0_T_SecR</t>
+  </si>
+  <si>
+    <t>VarboundSetFraction</t>
+  </si>
+  <si>
+    <t>HypercubicLengthFraction</t>
   </si>
 </sst>
 </file>
@@ -158,7 +471,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -243,11 +556,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -266,6 +590,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -281,6 +606,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Reactor_r10_analysis" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -548,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,9 +1557,14 @@
         <v>3</v>
       </c>
       <c r="E38" s="13">
-        <v>1</v>
-      </c>
-      <c r="F38" s="2"/>
+        <v>2.7933845999999998E-2</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>7485.76</v>
+      </c>
       <c r="J38">
         <v>15</v>
       </c>
@@ -1241,11 +1575,16 @@
         <v>10</v>
       </c>
       <c r="E39" s="13">
-        <v>1</v>
-      </c>
-      <c r="F39" s="2"/>
+        <v>2.6499796133723733E-2</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>16955.16</v>
+      </c>
       <c r="J39">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -1254,11 +1593,16 @@
         <v>50</v>
       </c>
       <c r="E40" s="13">
-        <v>1</v>
-      </c>
-      <c r="F40" s="2"/>
+        <v>2.6508390050616337E-2</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>17696.72</v>
+      </c>
       <c r="J40">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -1267,14 +1611,16 @@
         <v>100</v>
       </c>
       <c r="E41" s="13">
-        <v>1</v>
-      </c>
-      <c r="F41" s="2"/>
+        <v>2.6481141428296436E-2</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0</v>
+      </c>
       <c r="G41">
-        <v>7485.76</v>
+        <v>19104.560000000001</v>
       </c>
       <c r="J41">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -1285,14 +1631,18 @@
         <v>500</v>
       </c>
       <c r="E42" s="14">
-        <v>1</v>
-      </c>
-      <c r="F42" s="10"/>
-      <c r="G42" s="3"/>
+        <v>2.6532224844169328E-2</v>
+      </c>
+      <c r="F42" s="10">
+        <v>0</v>
+      </c>
+      <c r="G42" s="18">
+        <v>58583.6</v>
+      </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
-      <c r="J42">
-        <v>15</v>
+      <c r="J42" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -1308,7 +1658,18 @@
       <c r="D43" s="1">
         <v>3</v>
       </c>
-      <c r="F43" s="2"/>
+      <c r="E43" s="13">
+        <v>0.65647502610599995</v>
+      </c>
+      <c r="F43" s="2">
+        <v>62</v>
+      </c>
+      <c r="G43">
+        <v>48807.67</v>
+      </c>
+      <c r="J43" s="9">
+        <v>20</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C44" s="2"/>
@@ -1342,4 +1703,1276 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C245"/>
+  <sheetViews>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1.7763568394000001E-7</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1.7763568394000001E-7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="12">
+        <v>1.73472347598E-9</v>
+      </c>
+      <c r="C5" s="12">
+        <v>1.73472347598E-9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="12">
+        <v>7.1054273576000002E-7</v>
+      </c>
+      <c r="C6" s="12">
+        <v>7.1054273576000002E-7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="12">
+        <v>7.1054273576000002E-7</v>
+      </c>
+      <c r="C7" s="12">
+        <v>7.1054273576000002E-7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="12">
+        <v>3.5527136788000001E-7</v>
+      </c>
+      <c r="C8" s="12">
+        <v>3.5527136788000001E-7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="12">
+        <v>1</v>
+      </c>
+      <c r="C9" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="12">
+        <v>3.3683819582300002E-4</v>
+      </c>
+      <c r="C10" s="12">
+        <v>3.3683819582300002E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11">
+        <v>0.01</v>
+      </c>
+      <c r="C11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12">
+        <v>0.74339999999999995</v>
+      </c>
+      <c r="C12">
+        <v>0.74339999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="12">
+        <v>0.47267682881599998</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0.47267682881599998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="12">
+        <v>3.3267678750099998E-2</v>
+      </c>
+      <c r="C14" s="12">
+        <v>3.3267678750099998E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="12">
+        <v>0.63305156250000005</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0.63305156250000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18">
+        <v>0.42203437500000002</v>
+      </c>
+      <c r="C18">
+        <v>0.42203437500000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19">
+        <v>0.26785349925800001</v>
+      </c>
+      <c r="C19">
+        <v>0.26785349925800001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20">
+        <v>5.5869813368099999E-2</v>
+      </c>
+      <c r="C20">
+        <v>5.5869813368099999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21">
+        <v>0.95527707701200004</v>
+      </c>
+      <c r="C21">
+        <v>0.95527707701200004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22">
+        <v>0.11089226250000001</v>
+      </c>
+      <c r="C22">
+        <v>0.11089226250000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23">
+        <v>5.4850258718500003E-3</v>
+      </c>
+      <c r="C23">
+        <v>5.4850258718500003E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24">
+        <v>3.90099038285E-3</v>
+      </c>
+      <c r="C24">
+        <v>3.90099038285E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25">
+        <v>0.14471229664499999</v>
+      </c>
+      <c r="C25">
+        <v>0.14471229664499999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="12">
+        <v>0.187914216311</v>
+      </c>
+      <c r="C26" s="12">
+        <v>0.187914216311</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27">
+        <v>4.5485315373500002E-3</v>
+      </c>
+      <c r="C27">
+        <v>4.5485315373500002E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="12">
+        <v>5.5511151231299999E-7</v>
+      </c>
+      <c r="C28" s="12">
+        <v>5.5511151231299999E-7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="12">
+        <v>1.1102230246300001E-6</v>
+      </c>
+      <c r="C29" s="12">
+        <v>1.1102230246300001E-6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="12">
+        <v>2.2204460492500001E-6</v>
+      </c>
+      <c r="C30" s="12">
+        <v>2.2204460492500001E-6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="12">
+        <v>4.4408920984999999E-7</v>
+      </c>
+      <c r="C31" s="12">
+        <v>4.4408920984999999E-7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="12">
+        <v>5.5511151231299999E-7</v>
+      </c>
+      <c r="C32" s="12">
+        <v>5.5511151231299999E-7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="12">
+        <v>1</v>
+      </c>
+      <c r="C33" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="12">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="12">
+        <v>6.7762635780300003E-7</v>
+      </c>
+      <c r="C35" s="12">
+        <v>6.7762635780300003E-7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="12">
+        <v>6.7762635780300003E-7</v>
+      </c>
+      <c r="C36" s="12">
+        <v>6.7762635780300003E-7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="12">
+        <v>1.35525271561E-6</v>
+      </c>
+      <c r="C37" s="12">
+        <v>1.35525271561E-6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="12">
+        <v>1.35525271561E-6</v>
+      </c>
+      <c r="C38" s="12">
+        <v>1.35525271561E-6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="12">
+        <v>3.3881317890199997E-7</v>
+      </c>
+      <c r="C39" s="12">
+        <v>3.3881317890199997E-7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="12">
+        <v>0.72222222222200005</v>
+      </c>
+      <c r="C40" s="12">
+        <v>0.72222222222200005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="12">
+        <v>1.11022302463E-5</v>
+      </c>
+      <c r="C42" s="12">
+        <v>1.11022302463E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="12">
+        <v>5.5511151231300001E-6</v>
+      </c>
+      <c r="C43" s="12">
+        <v>5.5511151231300001E-6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="12">
+        <v>1.11022302463E-5</v>
+      </c>
+      <c r="C44" s="12">
+        <v>1.11022302463E-5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="12">
+        <v>1.11022302463E-5</v>
+      </c>
+      <c r="C45" s="12">
+        <v>1.11022302463E-5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="12">
+        <v>1.11022302463E-5</v>
+      </c>
+      <c r="C46" s="12">
+        <v>1.11022302463E-5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="C47" s="12">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48">
+        <v>0.15</v>
+      </c>
+      <c r="C48">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49">
+        <v>0.15</v>
+      </c>
+      <c r="C49">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50">
+        <v>0.15</v>
+      </c>
+      <c r="C50">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51">
+        <v>0.15</v>
+      </c>
+      <c r="C51">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52">
+        <v>3.9203074897700002E-2</v>
+      </c>
+      <c r="C52">
+        <v>3.9203074897700002E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53">
+        <v>3.1537098168400002E-2</v>
+      </c>
+      <c r="C53">
+        <v>3.1537098168400002E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54">
+        <v>0.75839999999999996</v>
+      </c>
+      <c r="C54">
+        <v>0.75839999999999996</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55">
+        <v>0.74340000047599997</v>
+      </c>
+      <c r="C55">
+        <v>0.74340000047599997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56">
+        <v>0.74582904406499995</v>
+      </c>
+      <c r="C56">
+        <v>0.74582904406499995</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57">
+        <v>0.74339999999999995</v>
+      </c>
+      <c r="C57">
+        <v>0.74339999999999995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>89</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>91</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>92</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>93</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>94</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>95</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>96</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>97</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>98</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>99</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>100</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>101</v>
+      </c>
+      <c r="B70">
+        <v>0.83785534371799997</v>
+      </c>
+      <c r="C70">
+        <v>0.83785534371799997</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>102</v>
+      </c>
+      <c r="B71" s="12">
+        <v>1.7763568394E-8</v>
+      </c>
+      <c r="C71" s="12">
+        <v>1.7763568394E-8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>103</v>
+      </c>
+      <c r="B72" s="12">
+        <v>4.7333671874999997E-2</v>
+      </c>
+      <c r="C72" s="12">
+        <v>4.7333671874999997E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>104</v>
+      </c>
+      <c r="B73">
+        <v>3.6008437499999997E-2</v>
+      </c>
+      <c r="C73">
+        <v>3.6008437499999997E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>105</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>106</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>107</v>
+      </c>
+      <c r="B76" s="12">
+        <v>9387731.5521200001</v>
+      </c>
+      <c r="C76" s="12">
+        <v>9387731.5521200001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>108</v>
+      </c>
+      <c r="B77" s="12">
+        <v>6.9602661929699994E-2</v>
+      </c>
+      <c r="C77" s="12">
+        <v>6.9602661929699994E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>109</v>
+      </c>
+      <c r="B78">
+        <v>5.3093453273800002E-2</v>
+      </c>
+      <c r="C78">
+        <v>5.3093453273800002E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>110</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>111</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>112</v>
+      </c>
+      <c r="B81">
+        <v>1.3861572369900001E-4</v>
+      </c>
+      <c r="C81">
+        <v>1.3861572369900001E-4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>113</v>
+      </c>
+      <c r="B82">
+        <v>2.22689900547E-2</v>
+      </c>
+      <c r="C82">
+        <v>2.22689900547E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>114</v>
+      </c>
+      <c r="B83">
+        <v>1.7085015773799998E-2</v>
+      </c>
+      <c r="C83">
+        <v>1.7085015773799998E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>115</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>116</v>
+      </c>
+      <c r="B85" s="12">
+        <v>1</v>
+      </c>
+      <c r="C85" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>117</v>
+      </c>
+      <c r="B86" s="12">
+        <v>4473840.8178099999</v>
+      </c>
+      <c r="C86" s="12">
+        <v>4473840.8178099999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>118</v>
+      </c>
+      <c r="B87" s="12">
+        <v>1</v>
+      </c>
+      <c r="C87" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>119</v>
+      </c>
+      <c r="B88" s="12">
+        <v>0.46486443807400002</v>
+      </c>
+      <c r="C88" s="12">
+        <v>0.46486443807400002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>120</v>
+      </c>
+      <c r="B89" s="12">
+        <v>190734.863281</v>
+      </c>
+      <c r="C89" s="12">
+        <v>190734.863281</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>121</v>
+      </c>
+      <c r="B90" s="12">
+        <v>1</v>
+      </c>
+      <c r="C90" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>122</v>
+      </c>
+      <c r="B91" s="12">
+        <v>7458675.0000099996</v>
+      </c>
+      <c r="C91" s="12">
+        <v>7458675.0000099996</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>123</v>
+      </c>
+      <c r="B92" s="12">
+        <v>7.9244999999999996E-2</v>
+      </c>
+      <c r="C92" s="12">
+        <v>7.9244999999999996E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>124</v>
+      </c>
+      <c r="B93" s="12">
+        <v>1.051575E-4</v>
+      </c>
+      <c r="C93" s="12">
+        <v>1.051575E-4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>125</v>
+      </c>
+      <c r="B94">
+        <v>1.2153E-4</v>
+      </c>
+      <c r="C94">
+        <v>1.2153E-4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>126</v>
+      </c>
+      <c r="B95" s="12">
+        <v>39326.250011099997</v>
+      </c>
+      <c r="C95" s="12">
+        <v>39326.250011099997</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>127</v>
+      </c>
+      <c r="B96" s="12">
+        <v>1</v>
+      </c>
+      <c r="C96" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>128</v>
+      </c>
+      <c r="B98">
+        <f>PRODUCT(B4:B96)</f>
+        <v>2.299087798858005E-147</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>129</v>
+      </c>
+      <c r="B99">
+        <f>B98^(1/93)</f>
+        <v>2.6499796133723733E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B109" s="12"/>
+      <c r="C109" s="12"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B110" s="12"/>
+      <c r="C110" s="12"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B111" s="12"/>
+      <c r="C111" s="12"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B112" s="12"/>
+      <c r="C112" s="12"/>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B113" s="12"/>
+      <c r="C113" s="12"/>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B116" s="12"/>
+      <c r="C116" s="12"/>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B117" s="12"/>
+      <c r="C117" s="12"/>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B118" s="12"/>
+      <c r="C118" s="12"/>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B119" s="12"/>
+      <c r="C119" s="12"/>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120" s="12"/>
+      <c r="C120" s="12"/>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B123" s="12"/>
+      <c r="C123" s="12"/>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B124" s="12"/>
+      <c r="C124" s="12"/>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B125" s="12"/>
+      <c r="C125" s="12"/>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B126" s="12"/>
+      <c r="C126" s="12"/>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B127" s="12"/>
+      <c r="C127" s="12"/>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B152" s="12"/>
+      <c r="C152" s="12"/>
+    </row>
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B154" s="12"/>
+      <c r="C154" s="12"/>
+    </row>
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B155" s="12"/>
+      <c r="C155" s="12"/>
+    </row>
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B156" s="12"/>
+      <c r="C156" s="12"/>
+    </row>
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B157" s="12"/>
+      <c r="C157" s="12"/>
+    </row>
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B158" s="12"/>
+      <c r="C158" s="12"/>
+    </row>
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B167" s="12"/>
+      <c r="C167" s="12"/>
+    </row>
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B170" s="12"/>
+      <c r="C170" s="12"/>
+    </row>
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B172" s="12"/>
+      <c r="C172" s="12"/>
+    </row>
+    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B173" s="12"/>
+      <c r="C173" s="12"/>
+    </row>
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B176" s="12"/>
+      <c r="C176" s="12"/>
+    </row>
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B178" s="12"/>
+      <c r="C178" s="12"/>
+    </row>
+    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B179" s="12"/>
+      <c r="C179" s="12"/>
+    </row>
+    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B180" s="12"/>
+      <c r="C180" s="12"/>
+    </row>
+    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B181" s="12"/>
+      <c r="C181" s="12"/>
+    </row>
+    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B182" s="12"/>
+      <c r="C182" s="12"/>
+    </row>
+    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B185" s="12"/>
+      <c r="C185" s="12"/>
+    </row>
+    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B186" s="12"/>
+      <c r="C186" s="12"/>
+    </row>
+    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B187" s="12"/>
+      <c r="C187" s="12"/>
+    </row>
+    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B188" s="12"/>
+      <c r="C188" s="12"/>
+    </row>
+    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B189" s="12"/>
+      <c r="C189" s="12"/>
+    </row>
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B192" s="12"/>
+      <c r="C192" s="12"/>
+    </row>
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B193" s="12"/>
+      <c r="C193" s="12"/>
+    </row>
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B194" s="12"/>
+      <c r="C194" s="12"/>
+    </row>
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B195" s="12"/>
+      <c r="C195" s="12"/>
+    </row>
+    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B196" s="12"/>
+      <c r="C196" s="12"/>
+    </row>
+    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B221" s="12"/>
+      <c r="C221" s="12"/>
+    </row>
+    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B226" s="12"/>
+      <c r="C226" s="12"/>
+    </row>
+    <row r="236" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B236" s="12"/>
+      <c r="C236" s="12"/>
+    </row>
+    <row r="239" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B239" s="12"/>
+      <c r="C239" s="12"/>
+    </row>
+    <row r="241" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B241" s="12"/>
+      <c r="C241" s="12"/>
+    </row>
+    <row r="242" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B242" s="12"/>
+      <c r="C242" s="12"/>
+    </row>
+    <row r="245" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B245" s="12"/>
+      <c r="C245" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>